<commit_message>
13.07.2020 MC sales Details
</commit_message>
<xml_diff>
--- a/2020/July/All Details/12.07.2020/MC Balance Transfer July 2020.xlsx
+++ b/2020/July/All Details/12.07.2020/MC Balance Transfer July 2020.xlsx
@@ -1174,7 +1174,7 @@
         <xdr:cNvPr id="1317" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1186,7 +1186,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1209,14 +1209,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1524,9 +1524,9 @@
   <dimension ref="A1:BI231"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="E70" sqref="E70"/>
+      <selection pane="bottomLeft" activeCell="D105" sqref="D105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -2498,14 +2498,14 @@
         <v>285750</v>
       </c>
       <c r="C14" s="2">
-        <v>293235</v>
+        <v>292035</v>
       </c>
       <c r="D14" s="2">
-        <v>630</v>
+        <v>830</v>
       </c>
       <c r="E14" s="2">
         <f t="shared" si="0"/>
-        <v>293865</v>
+        <v>292865</v>
       </c>
       <c r="F14" s="96"/>
       <c r="G14" s="17"/>
@@ -3798,19 +3798,19 @@
       </c>
       <c r="C33" s="2">
         <f>SUM(C5:C32)</f>
-        <v>5292550</v>
+        <v>5291350</v>
       </c>
       <c r="D33" s="2">
         <f>SUM(D5:D32)</f>
-        <v>12320</v>
+        <v>12520</v>
       </c>
       <c r="E33" s="2">
         <f>SUM(E5:E32)</f>
-        <v>5304870</v>
+        <v>5303870</v>
       </c>
       <c r="F33" s="67">
         <f>B33-E33</f>
-        <v>-511370</v>
+        <v>-510370</v>
       </c>
       <c r="G33" s="81"/>
       <c r="H33" s="86"/>
@@ -4081,10 +4081,10 @@
         <v>23</v>
       </c>
       <c r="C37" s="2">
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="E37" s="6"/>
       <c r="F37" s="95"/>
@@ -8558,7 +8558,7 @@
       <c r="B98" s="145"/>
       <c r="C98" s="32">
         <f>SUM(C37:C97)</f>
-        <v>1561293</v>
+        <v>1562293</v>
       </c>
       <c r="D98" s="28"/>
       <c r="F98" s="110"/>
@@ -8713,7 +8713,7 @@
       <c r="B100" s="143"/>
       <c r="C100" s="29">
         <f>C98+L121</f>
-        <v>1561293</v>
+        <v>1562293</v>
       </c>
       <c r="D100" s="21"/>
       <c r="F100" s="48"/>

</xml_diff>